<commit_message>
content: add data for Manhattan
</commit_message>
<xml_diff>
--- a/galleries.xlsx
+++ b/galleries.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yauheniya/Documents/03PRO/GitHubProjects/art-nyc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0CDE633-276C-1545-BF70-F9EFBA6ED368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7F584E-9E6D-4448-A5D4-A9825DFDCDD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{893F5228-64B7-F94C-9A14-47FC1D184A62}"/>
+    <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{893F5228-64B7-F94C-9A14-47FC1D184A62}"/>
   </bookViews>
   <sheets>
     <sheet name="Queens" sheetId="1" r:id="rId1"/>
     <sheet name="Bronx" sheetId="2" r:id="rId2"/>
     <sheet name="Brooklyn" sheetId="3" r:id="rId3"/>
+    <sheet name="Manhattan" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="588">
   <si>
     <t>Gallery Name</t>
   </si>
@@ -1190,13 +1191,625 @@
   </si>
   <si>
     <t>https://www.brooklynwayfarers.org</t>
+  </si>
+  <si>
+    <t>Gagosian</t>
+  </si>
+  <si>
+    <t>555 W 24th St, New York, NY 10011</t>
+  </si>
+  <si>
+    <t>info@gagosian.com</t>
+  </si>
+  <si>
+    <t>https://gagosian.com</t>
+  </si>
+  <si>
+    <t>David Zwirner</t>
+  </si>
+  <si>
+    <t>525 W 19th St, New York, NY 10011</t>
+  </si>
+  <si>
+    <t>info@davidzwirner.com</t>
+  </si>
+  <si>
+    <t>https://davidzwirner.com</t>
+  </si>
+  <si>
+    <t>Pace Gallery</t>
+  </si>
+  <si>
+    <t>540 W 25th St, New York, NY 10001</t>
+  </si>
+  <si>
+    <t>info@pacegallery.com</t>
+  </si>
+  <si>
+    <t>Gladstone Gallery</t>
+  </si>
+  <si>
+    <t>515 W 24th St, New York, NY 10011</t>
+  </si>
+  <si>
+    <t>info@gladstonegallery.com</t>
+  </si>
+  <si>
+    <t>https://gladstonegallery.com</t>
+  </si>
+  <si>
+    <t>Hauser &amp; Wirth</t>
+  </si>
+  <si>
+    <t>548 W 22nd St, New York, NY 10011</t>
+  </si>
+  <si>
+    <t>newyork@hauserwirth.com</t>
+  </si>
+  <si>
+    <t>https://hauserwirth.com</t>
+  </si>
+  <si>
+    <t>Marian Goodman Gallery</t>
+  </si>
+  <si>
+    <t>24 W 57th St, New York, NY 10019</t>
+  </si>
+  <si>
+    <t>info@mariangoodman.com</t>
+  </si>
+  <si>
+    <t>https://mariangoodman.com</t>
+  </si>
+  <si>
+    <t>Matthew Marks Gallery</t>
+  </si>
+  <si>
+    <t>523 W 24th St, New York, NY 10011</t>
+  </si>
+  <si>
+    <t>info@matthewmarks.com</t>
+  </si>
+  <si>
+    <t>https://matthewmarks.com</t>
+  </si>
+  <si>
+    <t>Jack Shainman Gallery</t>
+  </si>
+  <si>
+    <t>513 W 20th St, New York, NY 10011</t>
+  </si>
+  <si>
+    <t>info@jackshainman.com</t>
+  </si>
+  <si>
+    <t>https://jackshainman.com</t>
+  </si>
+  <si>
+    <t>Sean Kelly Gallery</t>
+  </si>
+  <si>
+    <t>475 10th Ave, New York, NY 10018</t>
+  </si>
+  <si>
+    <t>info@skny.com</t>
+  </si>
+  <si>
+    <t>https://skny.com</t>
+  </si>
+  <si>
+    <t>Lehmann Maupin</t>
+  </si>
+  <si>
+    <t>501 W 24th St, New York, NY 10011</t>
+  </si>
+  <si>
+    <t>info@lehmannmaupin.com</t>
+  </si>
+  <si>
+    <t>https://lehmannmaupin.com</t>
+  </si>
+  <si>
+    <t>Petzel Gallery</t>
+  </si>
+  <si>
+    <t>456 W 18th St, New York, NY 10011</t>
+  </si>
+  <si>
+    <t>info@petzel.com</t>
+  </si>
+  <si>
+    <t>https://petzel.com</t>
+  </si>
+  <si>
+    <t>Tanya Bonakdar Gallery</t>
+  </si>
+  <si>
+    <t>521 W 21st St, New York, NY 10011</t>
+  </si>
+  <si>
+    <t>info@tanyabonakdargallery.com</t>
+  </si>
+  <si>
+    <t>https://tanyabonakdargallery.com</t>
+  </si>
+  <si>
+    <t>Paula Cooper Gallery</t>
+  </si>
+  <si>
+    <t>534 W 21st St, New York, NY 10011</t>
+  </si>
+  <si>
+    <t>info@paulacoopergallery.com</t>
+  </si>
+  <si>
+    <t>https://paulacoopergallery.com</t>
+  </si>
+  <si>
+    <t>303 Gallery</t>
+  </si>
+  <si>
+    <t>555 W 21st St, New York, NY 10011</t>
+  </si>
+  <si>
+    <t>info@303gallery.com</t>
+  </si>
+  <si>
+    <t>Andrew Kreps Gallery</t>
+  </si>
+  <si>
+    <t>22 Cortlandt Alley, New York, NY 10013</t>
+  </si>
+  <si>
+    <t>info@andrewkreps.com</t>
+  </si>
+  <si>
+    <t>Bortolami Gallery</t>
+  </si>
+  <si>
+    <t>39 Walker St, New York, NY 10013</t>
+  </si>
+  <si>
+    <t>info@bortolamigallery.com</t>
+  </si>
+  <si>
+    <t>https://bortolamigallery.com</t>
+  </si>
+  <si>
+    <t>James Cohan Gallery</t>
+  </si>
+  <si>
+    <t>48 Walker St, New York, NY 10013</t>
+  </si>
+  <si>
+    <t>info@jamescohan.com</t>
+  </si>
+  <si>
+    <t>https://jamescohan.com</t>
+  </si>
+  <si>
+    <t>Sikkema Jenkins &amp; Co.</t>
+  </si>
+  <si>
+    <t>530 W 22nd St, New York, NY 10011</t>
+  </si>
+  <si>
+    <t>info@sikkemajenkinsco.com</t>
+  </si>
+  <si>
+    <t>https://sikkemajenkinsco.com</t>
+  </si>
+  <si>
+    <t>Lisson Gallery</t>
+  </si>
+  <si>
+    <t>504 W 24th St, New York, NY 10011</t>
+  </si>
+  <si>
+    <t>info@lissongallery.com</t>
+  </si>
+  <si>
+    <t>https://lissongallery.com</t>
+  </si>
+  <si>
+    <t>Yossi Milo Gallery</t>
+  </si>
+  <si>
+    <t>245 Tenth Ave, New York, NY 10001</t>
+  </si>
+  <si>
+    <t>info@yossimilo.com</t>
+  </si>
+  <si>
+    <t>https://yossimilo.com</t>
+  </si>
+  <si>
+    <t>Luhring Augustine</t>
+  </si>
+  <si>
+    <t>531 W 24th St, New York, NY 10011</t>
+  </si>
+  <si>
+    <t>info@luhringaugustine.com</t>
+  </si>
+  <si>
+    <t>https://luhringaugustine.com</t>
+  </si>
+  <si>
+    <t>David Kordansky Gallery</t>
+  </si>
+  <si>
+    <t>520 W 20th St, New York, NY 10011</t>
+  </si>
+  <si>
+    <t>info@davidkordanskygallery.com</t>
+  </si>
+  <si>
+    <t>https://davidkordanskygallery.com</t>
+  </si>
+  <si>
+    <t>Kasmin Gallery</t>
+  </si>
+  <si>
+    <t>509 W 27th St, New York, NY 10001</t>
+  </si>
+  <si>
+    <t>info@kasmingallery.com</t>
+  </si>
+  <si>
+    <t>https://kasmingallery.com</t>
+  </si>
+  <si>
+    <t>Anton Kern Gallery</t>
+  </si>
+  <si>
+    <t>16 E 55th St, New York, NY 10022</t>
+  </si>
+  <si>
+    <t>info@antonkerngallery.com</t>
+  </si>
+  <si>
+    <t>https://antonkerngallery.com</t>
+  </si>
+  <si>
+    <t>Alexander Gray Associates</t>
+  </si>
+  <si>
+    <t>510 W 26th St, New York, NY 10001</t>
+  </si>
+  <si>
+    <t>info@alexandergray.com</t>
+  </si>
+  <si>
+    <t>https://alexandergray.com</t>
+  </si>
+  <si>
+    <t>Galerie Lelong &amp; Co.</t>
+  </si>
+  <si>
+    <t>528 W 26th St, New York, NY 10001</t>
+  </si>
+  <si>
+    <t>info@galerielelong.com</t>
+  </si>
+  <si>
+    <t>https://galerielelong.com</t>
+  </si>
+  <si>
+    <t>Cheim &amp; Read</t>
+  </si>
+  <si>
+    <t>23 E 67th St, New York, NY 10065</t>
+  </si>
+  <si>
+    <t>info@cheimread.com</t>
+  </si>
+  <si>
+    <t>https://cheimread.com</t>
+  </si>
+  <si>
+    <t>Marianne Boesky Gallery</t>
+  </si>
+  <si>
+    <t>507 W 24th St, New York, NY 10011</t>
+  </si>
+  <si>
+    <t>info@boeskygallery.com</t>
+  </si>
+  <si>
+    <t>Metro Pictures</t>
+  </si>
+  <si>
+    <t>519 W 24th St, New York, NY 10011</t>
+  </si>
+  <si>
+    <t>info@metropictures.com</t>
+  </si>
+  <si>
+    <t>https://metropictures.com</t>
+  </si>
+  <si>
+    <t>Greene Naftali</t>
+  </si>
+  <si>
+    <t>508 W 26th St, New York, NY 10001</t>
+  </si>
+  <si>
+    <t>info@greenenaftaligallery.com</t>
+  </si>
+  <si>
+    <t>https://greenenaftaligallery.com</t>
+  </si>
+  <si>
+    <t>Mitchell-Innes &amp; Nash</t>
+  </si>
+  <si>
+    <t>534 W 26th St, New York, NY 10001</t>
+  </si>
+  <si>
+    <t>info@miandn.com</t>
+  </si>
+  <si>
+    <t>https://miandn.com</t>
+  </si>
+  <si>
+    <t>Casey Kaplan Gallery</t>
+  </si>
+  <si>
+    <t>121 W 27th St, New York, NY 10001</t>
+  </si>
+  <si>
+    <t>info@caseykaplangallery.com</t>
+  </si>
+  <si>
+    <t>https://caseykaplangallery.com</t>
+  </si>
+  <si>
+    <t>Jack Hanley Gallery</t>
+  </si>
+  <si>
+    <t>327 Broome St, New York, NY 10002</t>
+  </si>
+  <si>
+    <t>info@jackhanley.com</t>
+  </si>
+  <si>
+    <t>https://jackhanley.com</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>60 Lispenard St, New York, NY 10013</t>
+  </si>
+  <si>
+    <t>info@canadanewyork.com</t>
+  </si>
+  <si>
+    <t>https://canadanewyork.com</t>
+  </si>
+  <si>
+    <t>Karma</t>
+  </si>
+  <si>
+    <t>188 E 2nd St, New York, NY 10009</t>
+  </si>
+  <si>
+    <t>info@karmakarma.org</t>
+  </si>
+  <si>
+    <t>https://karmakarma.org</t>
+  </si>
+  <si>
+    <t>Nicelle Beauchene Gallery</t>
+  </si>
+  <si>
+    <t>7 Franklin Pl, New York, NY 10013</t>
+  </si>
+  <si>
+    <t>info@nicellebeauchene.com</t>
+  </si>
+  <si>
+    <t>https://nicellebeauchene.com</t>
+  </si>
+  <si>
+    <t>PPOW Gallery</t>
+  </si>
+  <si>
+    <t>392 Broadway, New York, NY 10013</t>
+  </si>
+  <si>
+    <t>info@ppowgallery.com</t>
+  </si>
+  <si>
+    <t>https://ppowgallery.com</t>
+  </si>
+  <si>
+    <t>The Hole</t>
+  </si>
+  <si>
+    <t>312 Bowery, New York, NY 10012</t>
+  </si>
+  <si>
+    <t>info@theholenyc.com</t>
+  </si>
+  <si>
+    <t>https://theholenyc.com</t>
+  </si>
+  <si>
+    <t>Rachel Uffner Gallery</t>
+  </si>
+  <si>
+    <t>170 Suffolk St, New York, NY 10002</t>
+  </si>
+  <si>
+    <t>info@racheluffnergallery.com</t>
+  </si>
+  <si>
+    <t>https://racheluffnergallery.com</t>
+  </si>
+  <si>
+    <t>Jeffrey Deitch Gallery</t>
+  </si>
+  <si>
+    <t>18 Wooster St, New York, NY 10013</t>
+  </si>
+  <si>
+    <t>info@deitch.com</t>
+  </si>
+  <si>
+    <t>https://deitch.com</t>
+  </si>
+  <si>
+    <t>Marlborough Gallery</t>
+  </si>
+  <si>
+    <t>545 W 25th St, New York, NY 10001</t>
+  </si>
+  <si>
+    <t>info@marlboroughgallery.com</t>
+  </si>
+  <si>
+    <t>https://marlboroughgallery.com</t>
+  </si>
+  <si>
+    <t>Skarstedt Gallery</t>
+  </si>
+  <si>
+    <t>550 W 21st St, New York, NY 10011</t>
+  </si>
+  <si>
+    <t>info@skarstedt.com</t>
+  </si>
+  <si>
+    <t>https://skarstedt.com</t>
+  </si>
+  <si>
+    <t>Fergus McCaffrey</t>
+  </si>
+  <si>
+    <t>514 W 26th St, New York, NY 10001</t>
+  </si>
+  <si>
+    <t>info@fergusmccaffrey.com</t>
+  </si>
+  <si>
+    <t>https://fergusmccaffrey.com</t>
+  </si>
+  <si>
+    <t>Venus Over Manhattan</t>
+  </si>
+  <si>
+    <t>55 Great Jones St, New York, NY 10012</t>
+  </si>
+  <si>
+    <t>info@venusovermanhattan.com</t>
+  </si>
+  <si>
+    <t>https://venusovermanhattan.com</t>
+  </si>
+  <si>
+    <t>David Nolan Gallery</t>
+  </si>
+  <si>
+    <t>24 E 81st St, New York, NY 10028</t>
+  </si>
+  <si>
+    <t>info@davidnolangallery.com</t>
+  </si>
+  <si>
+    <t>https://davidnolangallery.com</t>
+  </si>
+  <si>
+    <t>Sapar Contemporary</t>
+  </si>
+  <si>
+    <t>9 N Moore St, New York, NY 10013</t>
+  </si>
+  <si>
+    <t>info@saparcontemporary.com</t>
+  </si>
+  <si>
+    <t>https://saparcontemporary.com</t>
+  </si>
+  <si>
+    <t>Bodega</t>
+  </si>
+  <si>
+    <t>167 Rivington St, New York, NY 10002</t>
+  </si>
+  <si>
+    <t>info@bodega-us.org</t>
+  </si>
+  <si>
+    <t>https://bodega-us.org</t>
+  </si>
+  <si>
+    <t>Lyles &amp; King</t>
+  </si>
+  <si>
+    <t>21 Catherine St, New York, NY 10038</t>
+  </si>
+  <si>
+    <t>info@lylesandking.com</t>
+  </si>
+  <si>
+    <t>https://lylesandking.com</t>
+  </si>
+  <si>
+    <t>Fort Gansevoort</t>
+  </si>
+  <si>
+    <t>5 Ninth Ave, New York, NY 10014</t>
+  </si>
+  <si>
+    <t>info@fortgansevoort.com</t>
+  </si>
+  <si>
+    <t>https://fortgansevoort.com</t>
+  </si>
+  <si>
+    <t>Albertz Benda</t>
+  </si>
+  <si>
+    <t>515 W 26th St, New York, NY 10001</t>
+  </si>
+  <si>
+    <t>info@albertzbenda.com</t>
+  </si>
+  <si>
+    <t>https://albertzbenda.com</t>
+  </si>
+  <si>
+    <t>Simone Subal Gallery</t>
+  </si>
+  <si>
+    <t>131 Bowery, New York, NY 10002</t>
+  </si>
+  <si>
+    <t>info@simonesubal.com</t>
+  </si>
+  <si>
+    <t>https://simonesubal.com</t>
+  </si>
+  <si>
+    <t>https://www.pacegallery.com</t>
+  </si>
+  <si>
+    <t>https://www.303gallery.com</t>
+  </si>
+  <si>
+    <t>http://www.andrewkreps.com</t>
+  </si>
+  <si>
+    <t>https://marianneboeskygallery.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1227,6 +1840,11 @@
       <color theme="1"/>
       <name val="Roboto"/>
     </font>
+    <font>
+      <sz val="10.5"/>
+      <color theme="1"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1249,12 +1867,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2552,8 +3171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DE7FBF8-CFF9-7B4E-868E-2E1E1B9DDB04}">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D28" sqref="A28:D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3344,4 +3963,863 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5B93F1E-8B8D-0A42-B108-519592BEC53A}">
+  <dimension ref="A1:D56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>467</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>475</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>483</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>494</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>518</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>522</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>542</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>550</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>554</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>558</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>570</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>573</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>574</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>578</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>582</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="17" x14ac:dyDescent="0.25">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="mailto:info@gagosian.com" xr:uid="{08F625F3-9B85-C342-B856-36453C9041FE}"/>
+    <hyperlink ref="D2" r:id="rId2" display="https://gagosian.com/" xr:uid="{BCCAFEA9-5E9A-8D4D-9B29-B6E79B3C0537}"/>
+    <hyperlink ref="C3" r:id="rId3" display="mailto:info@davidzwirner.com" xr:uid="{D7F666C3-B78A-034F-8939-EE33146F1659}"/>
+    <hyperlink ref="D3" r:id="rId4" display="https://davidzwirner.com/" xr:uid="{FDF8888A-A13A-D64F-BA41-63305A012FDC}"/>
+    <hyperlink ref="C4" r:id="rId5" display="mailto:info@pacegallery.com" xr:uid="{88F6BA6C-2511-9E41-A1FC-0F05AB0A0CFE}"/>
+    <hyperlink ref="D4" r:id="rId6" xr:uid="{F6F9E8D0-4708-064B-9082-6A6C703D9899}"/>
+    <hyperlink ref="C5" r:id="rId7" display="mailto:info@gladstonegallery.com" xr:uid="{6723A782-FC75-7844-A311-9A41BA89A0CE}"/>
+    <hyperlink ref="D5" r:id="rId8" display="https://gladstonegallery.com/" xr:uid="{6055C68C-2FD3-8D44-9A53-A10ABFC64FA0}"/>
+    <hyperlink ref="C6" r:id="rId9" display="mailto:newyork@hauserwirth.com" xr:uid="{036BAA26-B689-1E40-A552-88EEF6AA8ABE}"/>
+    <hyperlink ref="D6" r:id="rId10" display="https://hauserwirth.com/" xr:uid="{8DEEB515-DAC5-C04D-9C40-98E4B56481AF}"/>
+    <hyperlink ref="C7" r:id="rId11" display="mailto:info@mariangoodman.com" xr:uid="{FA1B6C2C-BECD-E545-8901-E6B71F1DBCA6}"/>
+    <hyperlink ref="D7" r:id="rId12" display="https://mariangoodman.com/" xr:uid="{88D232C6-01B9-F648-8DD4-A15CD42023EE}"/>
+    <hyperlink ref="C8" r:id="rId13" display="mailto:info@matthewmarks.com" xr:uid="{72CCCE91-42B1-CC4B-8B08-026090FB691E}"/>
+    <hyperlink ref="D8" r:id="rId14" display="https://matthewmarks.com/" xr:uid="{CDBFAF41-491D-9B46-AFB6-9A49522C8C21}"/>
+    <hyperlink ref="C9" r:id="rId15" display="mailto:info@jackshainman.com" xr:uid="{6CDBF0B2-EDEE-4D43-8CE5-CC991CBFA151}"/>
+    <hyperlink ref="D9" r:id="rId16" display="https://jackshainman.com/" xr:uid="{E31ADD06-FE04-9D4C-80D4-5C1794DF80E4}"/>
+    <hyperlink ref="C10" r:id="rId17" display="mailto:info@skny.com" xr:uid="{B49DC9F8-E5F1-094C-902A-1CBCA72F3422}"/>
+    <hyperlink ref="D10" r:id="rId18" display="https://skny.com/" xr:uid="{68CAA661-AE38-3B44-A8D2-EF562E522823}"/>
+    <hyperlink ref="C11" r:id="rId19" display="mailto:info@lehmannmaupin.com" xr:uid="{3E126C2D-51A0-B84E-8247-3B6C6DD7F049}"/>
+    <hyperlink ref="D11" r:id="rId20" display="https://lehmannmaupin.com/" xr:uid="{36D00D4B-B603-E646-8124-DB2ACBF4A100}"/>
+    <hyperlink ref="C12" r:id="rId21" display="mailto:info@petzel.com" xr:uid="{2814D3C5-C2F2-1C4C-BFF2-7207F2D29177}"/>
+    <hyperlink ref="D12" r:id="rId22" display="https://petzel.com/" xr:uid="{30B9743F-70A4-564F-BD2D-814B968CAB37}"/>
+    <hyperlink ref="C13" r:id="rId23" display="mailto:info@tanyabonakdargallery.com" xr:uid="{ED12B166-854B-A44F-9E85-6F0A356CDBE4}"/>
+    <hyperlink ref="D13" r:id="rId24" display="https://tanyabonakdargallery.com/" xr:uid="{E7932D1E-671E-084F-9937-5F8CC1C7EE33}"/>
+    <hyperlink ref="C14" r:id="rId25" display="mailto:info@paulacoopergallery.com" xr:uid="{4DD630A0-0CCE-1B4B-83C0-2E583D9832DF}"/>
+    <hyperlink ref="D14" r:id="rId26" display="https://paulacoopergallery.com/" xr:uid="{BF4CE405-C4FA-2F4A-B164-13B1F3947912}"/>
+    <hyperlink ref="C15" r:id="rId27" display="mailto:info@303gallery.com" xr:uid="{EFCB9A61-4437-5E41-B9AF-C6126F7E141B}"/>
+    <hyperlink ref="D15" r:id="rId28" xr:uid="{40A899D5-FAF3-A347-9090-1542D698148A}"/>
+    <hyperlink ref="C16" r:id="rId29" display="mailto:info@andrewkreps.com" xr:uid="{D87BC3E8-88FE-1649-9431-80A715742C8C}"/>
+    <hyperlink ref="D16" r:id="rId30" xr:uid="{5302223C-1436-0049-8CE9-6B028C55922E}"/>
+    <hyperlink ref="C17" r:id="rId31" display="mailto:info@bortolamigallery.com" xr:uid="{E5C4580B-92E9-9841-BA96-551170EEE094}"/>
+    <hyperlink ref="D17" r:id="rId32" display="https://bortolamigallery.com/" xr:uid="{100909A7-9F00-9848-80C5-5B11FB34B64B}"/>
+    <hyperlink ref="C18" r:id="rId33" display="mailto:info@jamescohan.com" xr:uid="{FF89514F-3121-134C-8D66-81B7E876C050}"/>
+    <hyperlink ref="D18" r:id="rId34" display="https://jamescohan.com/" xr:uid="{7528CC06-03AF-5F43-B222-CFA6F4D5DC3C}"/>
+    <hyperlink ref="C19" r:id="rId35" display="mailto:info@sikkemajenkinsco.com" xr:uid="{5CD4E0AD-D13F-2F4C-A25C-897011EF86C5}"/>
+    <hyperlink ref="D19" r:id="rId36" display="https://sikkemajenkinsco.com/" xr:uid="{167467A5-FB37-C44B-BE27-182333EA80F2}"/>
+    <hyperlink ref="C20" r:id="rId37" display="mailto:info@lissongallery.com" xr:uid="{D9B9F655-AAC4-344E-8D7F-A4809FB64148}"/>
+    <hyperlink ref="D20" r:id="rId38" display="https://lissongallery.com/" xr:uid="{F27D3172-A538-6443-A9F7-9313E9B87631}"/>
+    <hyperlink ref="C21" r:id="rId39" display="mailto:info@yossimilo.com" xr:uid="{D0E004B8-95BC-2549-B760-59B4D60172CC}"/>
+    <hyperlink ref="D21" r:id="rId40" display="https://yossimilo.com/" xr:uid="{E5ACF25B-C9D4-F345-837E-13E9E79F5790}"/>
+    <hyperlink ref="C22" r:id="rId41" display="mailto:info@luhringaugustine.com" xr:uid="{1089E6D6-6331-3545-9DD4-ADBFF5E2F663}"/>
+    <hyperlink ref="D22" r:id="rId42" display="https://luhringaugustine.com/" xr:uid="{650D8844-4000-354A-AF04-D10C597A0D3C}"/>
+    <hyperlink ref="C23" r:id="rId43" display="mailto:info@davidkordanskygallery.com" xr:uid="{25CFF424-D406-C44B-B53E-9234BC6F0020}"/>
+    <hyperlink ref="D23" r:id="rId44" display="https://davidkordanskygallery.com/" xr:uid="{A04A7FAB-C0F9-994E-AAC5-42E930693CA6}"/>
+    <hyperlink ref="C24" r:id="rId45" display="mailto:info@kasmingallery.com" xr:uid="{731162F5-31F4-1847-82F3-B65E3946EC4A}"/>
+    <hyperlink ref="D24" r:id="rId46" display="https://kasmingallery.com/" xr:uid="{40CAF0BE-56F4-E74E-A948-9965DDA339FE}"/>
+    <hyperlink ref="C25" r:id="rId47" display="mailto:info@antonkerngallery.com" xr:uid="{C804F52D-9F1F-A24E-95B7-4758898BA82D}"/>
+    <hyperlink ref="D25" r:id="rId48" display="https://antonkerngallery.com/" xr:uid="{0387CD21-8077-F148-9F07-E1E0E5696900}"/>
+    <hyperlink ref="C26" r:id="rId49" display="mailto:info@alexandergray.com" xr:uid="{33861A9D-C4FE-6140-85D3-68E3223F7381}"/>
+    <hyperlink ref="D26" r:id="rId50" display="https://alexandergray.com/" xr:uid="{6E43F5F2-0D7D-4849-A8A9-6257AE2F113E}"/>
+    <hyperlink ref="C27" r:id="rId51" display="mailto:info@galerielelong.com" xr:uid="{632C2DFE-1BE9-8E40-B7D4-0E8C000EBB8D}"/>
+    <hyperlink ref="D27" r:id="rId52" display="https://galerielelong.com/" xr:uid="{C8DB4721-9E2A-C14C-8414-B545F6542F5A}"/>
+    <hyperlink ref="C28" r:id="rId53" display="mailto:info@cheimread.com" xr:uid="{B8F0A7BE-0E1B-4E45-A1FF-FF3471859E03}"/>
+    <hyperlink ref="D28" r:id="rId54" display="https://cheimread.com/" xr:uid="{C6EA174B-377F-7F41-B50E-601575E43991}"/>
+    <hyperlink ref="C29" r:id="rId55" display="mailto:info@boeskygallery.com" xr:uid="{CEA8A9C9-C5F7-AF47-8836-5BD26A120DD0}"/>
+    <hyperlink ref="D29" r:id="rId56" xr:uid="{BD16CB51-1FA9-664A-8E9B-B0684EAE6B60}"/>
+    <hyperlink ref="C30" r:id="rId57" display="mailto:info@metropictures.com" xr:uid="{09A46D66-0E3D-0D45-A5A7-2C38FE20DB11}"/>
+    <hyperlink ref="D30" r:id="rId58" display="https://metropictures.com/" xr:uid="{846B45E7-5CC1-254D-8A46-1C98BC6603BC}"/>
+    <hyperlink ref="C31" r:id="rId59" display="mailto:info@greenenaftaligallery.com" xr:uid="{68761117-029D-C947-8C0B-A4F41AA67A30}"/>
+    <hyperlink ref="D31" r:id="rId60" display="https://greenenaftaligallery.com/" xr:uid="{646479D1-D542-D547-AE95-F7006A8048C1}"/>
+    <hyperlink ref="C32" r:id="rId61" display="mailto:info@miandn.com" xr:uid="{FD4E6451-533E-4841-82DA-163E289BF198}"/>
+    <hyperlink ref="D32" r:id="rId62" display="https://miandn.com/" xr:uid="{DC0F2A09-AB26-9241-847C-A0908D87D93A}"/>
+    <hyperlink ref="C33" r:id="rId63" display="mailto:info@caseykaplangallery.com" xr:uid="{AF224C76-9220-7041-B981-0258AD046B1D}"/>
+    <hyperlink ref="D33" r:id="rId64" display="https://caseykaplangallery.com/" xr:uid="{8BF53608-E28F-174F-A7E5-7FCD10FB5BCD}"/>
+    <hyperlink ref="C34" r:id="rId65" display="mailto:info@jackhanley.com" xr:uid="{FC044EA8-F9A4-A047-B06F-6A94FC98B93C}"/>
+    <hyperlink ref="D34" r:id="rId66" display="https://jackhanley.com/" xr:uid="{C54C421A-F7F1-5C4A-8B0A-D733FB4FD52E}"/>
+    <hyperlink ref="C35" r:id="rId67" display="mailto:info@canadanewyork.com" xr:uid="{7EA86D59-1D98-4746-BADA-592254A426A1}"/>
+    <hyperlink ref="D35" r:id="rId68" display="https://canadanewyork.com/" xr:uid="{7E92ADB5-19E5-3A43-A27C-AB2676D35E4F}"/>
+    <hyperlink ref="C36" r:id="rId69" display="mailto:info@karmakarma.org" xr:uid="{9034E3D1-9CCC-6447-A579-FA045593FCC4}"/>
+    <hyperlink ref="D36" r:id="rId70" display="https://karmakarma.org/" xr:uid="{4D80CD62-F2DA-CC48-99C1-7AD52C0B14A8}"/>
+    <hyperlink ref="C37" r:id="rId71" display="mailto:info@nicellebeauchene.com" xr:uid="{8D80DB20-B298-2E40-8F61-203CA8184E59}"/>
+    <hyperlink ref="D37" r:id="rId72" display="https://nicellebeauchene.com/" xr:uid="{A981373C-3C33-5B47-8EE8-5EBEC73F2D8F}"/>
+    <hyperlink ref="C38" r:id="rId73" display="mailto:info@ppowgallery.com" xr:uid="{297B189B-AF05-AD46-BABC-06DCF5A31447}"/>
+    <hyperlink ref="D38" r:id="rId74" display="https://ppowgallery.com/" xr:uid="{7BB54162-6110-884E-A0E9-CDD4B0BEA794}"/>
+    <hyperlink ref="C39" r:id="rId75" display="mailto:info@theholenyc.com" xr:uid="{DA0777A8-9321-6640-BBA1-1CFA50DC5B93}"/>
+    <hyperlink ref="D39" r:id="rId76" display="https://theholenyc.com/" xr:uid="{B5C36F03-35BA-6B49-9EBA-4D6C2E218B03}"/>
+    <hyperlink ref="C40" r:id="rId77" display="mailto:info@racheluffnergallery.com" xr:uid="{9BD87B95-CB85-3648-8926-D030617EB75D}"/>
+    <hyperlink ref="D40" r:id="rId78" display="https://racheluffnergallery.com/" xr:uid="{B37A4BBD-682F-434B-92A7-5FA711FAD20B}"/>
+    <hyperlink ref="C41" r:id="rId79" display="mailto:info@deitch.com" xr:uid="{371E067D-8326-3E49-97AA-9CCB3A810BCE}"/>
+    <hyperlink ref="D41" r:id="rId80" display="https://deitch.com/" xr:uid="{324ED483-2B34-5A41-9A0C-255D129088F5}"/>
+    <hyperlink ref="C42" r:id="rId81" display="mailto:info@marlboroughgallery.com" xr:uid="{C5005179-FF75-6D4E-A5B8-FF7515618402}"/>
+    <hyperlink ref="D42" r:id="rId82" display="https://marlboroughgallery.com/" xr:uid="{6B0F6444-DA7B-9243-8852-092EB44C131A}"/>
+    <hyperlink ref="C43" r:id="rId83" display="mailto:info@skarstedt.com" xr:uid="{BD35ADD5-8064-7B42-82D7-E49847312204}"/>
+    <hyperlink ref="D43" r:id="rId84" display="https://skarstedt.com/" xr:uid="{440BA55A-92B2-7244-9900-5ED6CD8DB240}"/>
+    <hyperlink ref="C44" r:id="rId85" display="mailto:info@fergusmccaffrey.com" xr:uid="{8051DA74-8AC0-B94B-80F6-4A94B0300EEB}"/>
+    <hyperlink ref="D44" r:id="rId86" display="https://fergusmccaffrey.com/" xr:uid="{9B285762-30EA-8049-B7DC-1465807CDF64}"/>
+    <hyperlink ref="C45" r:id="rId87" display="mailto:info@venusovermanhattan.com" xr:uid="{7D74F152-28A9-A74C-A3F3-F6B6982A06DB}"/>
+    <hyperlink ref="D45" r:id="rId88" display="https://venusovermanhattan.com/" xr:uid="{3188427B-4404-3347-93CC-4C4BF2FDF2DA}"/>
+    <hyperlink ref="C46" r:id="rId89" display="mailto:info@davidnolangallery.com" xr:uid="{1C4C3B36-83C7-4647-B708-D707D9AA4D9B}"/>
+    <hyperlink ref="D46" r:id="rId90" display="https://davidnolangallery.com/" xr:uid="{BC5C6F4F-B718-1D40-8A89-A5BF5760B94D}"/>
+    <hyperlink ref="C47" r:id="rId91" display="mailto:info@saparcontemporary.com" xr:uid="{BB6E77B4-7A9F-6049-A20D-E4CEE1F4B259}"/>
+    <hyperlink ref="D47" r:id="rId92" display="https://saparcontemporary.com/" xr:uid="{456A696F-515A-F64C-94EA-9D28A5527940}"/>
+    <hyperlink ref="C48" r:id="rId93" display="mailto:info@bodega-us.org" xr:uid="{D505D40B-383B-AC48-9F14-E02A5FA5F9E7}"/>
+    <hyperlink ref="D48" r:id="rId94" display="https://bodega-us.org/" xr:uid="{3F25E6BB-CB48-154A-9116-80549A293EBB}"/>
+    <hyperlink ref="C49" r:id="rId95" display="mailto:info@lylesandking.com" xr:uid="{FC4CE3F7-DA7E-6945-945C-8DDADE28CAE5}"/>
+    <hyperlink ref="D49" r:id="rId96" display="https://lylesandking.com/" xr:uid="{A4CD63EC-A1EB-3D49-928F-D543F81A96BF}"/>
+    <hyperlink ref="C50" r:id="rId97" display="mailto:info@fortgansevoort.com" xr:uid="{5E2E67BC-9C30-2C44-8599-A677C7BE0AB4}"/>
+    <hyperlink ref="D50" r:id="rId98" display="https://fortgansevoort.com/" xr:uid="{50E86941-3E2E-9B41-B12F-EA57B02F9DB6}"/>
+    <hyperlink ref="C51" r:id="rId99" display="mailto:info@albertzbenda.com" xr:uid="{7B5342E7-9897-2841-9E49-AA3BC224525D}"/>
+    <hyperlink ref="D51" r:id="rId100" display="https://albertzbenda.com/" xr:uid="{FE37C884-80E9-4147-A101-2F44EE5078EC}"/>
+    <hyperlink ref="C52" r:id="rId101" display="mailto:info@simonesubal.com" xr:uid="{14B0790E-C348-D54B-B1B3-85891EBD4729}"/>
+    <hyperlink ref="D52" r:id="rId102" display="https://simonesubal.com/" xr:uid="{49C88C63-9225-7E45-9B1B-5C342DDD5782}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>